<commit_message>
27-10-2018 excel and script
</commit_message>
<xml_diff>
--- a/excel writer/tut 1/Expenses01.xlsx
+++ b/excel writer/tut 1/Expenses01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Rent</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>kaka</t>
   </si>
 </sst>
 </file>
@@ -405,8 +402,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <f>SUM(B1:B4)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>